<commit_message>
updated my agile file
</commit_message>
<xml_diff>
--- a/Agile_Template_v0.1.xlsx
+++ b/Agile_Template_v0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AryanProgramming\InfosysFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6E8CD3-9CFA-4DE9-A668-EEDB9A64EC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7817147B-F677-4147-8BE8-9BBE367F4324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1134,7 +1134,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1511,7 +1511,7 @@
         <v>90</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
@@ -1535,7 +1535,7 @@
         <v>90</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">

</xml_diff>